<commit_message>
Finished AU and LU
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G54-0624-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G54-0624-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rico\Desktop\ENSC 350 Part1\ENSC350FP\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F230133F-F2A6-4766-ADC8-E4071AE932DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BC4DAA-52D8-430E-87C1-B3686ADEF6E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5730" yWindow="3495" windowWidth="21600" windowHeight="11385" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -74,9 +74,6 @@
     <t>"0624"</t>
   </si>
   <si>
-    <t>29/03/2020</t>
-  </si>
-  <si>
     <t>9:00pm</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>Helped my teammates set up Git and helped them with setting up of Quartus and ModelSim</t>
   </si>
   <si>
-    <t>30/03/2020</t>
-  </si>
-  <si>
     <t>11:00pm</t>
   </si>
   <si>
@@ -110,9 +104,6 @@
     <t>Finished the Logic Unit</t>
   </si>
   <si>
-    <t>31/03/2020</t>
-  </si>
-  <si>
     <t>7:59pm</t>
   </si>
   <si>
@@ -120,6 +111,24 @@
   </si>
   <si>
     <t>10:25pm</t>
+  </si>
+  <si>
+    <t>12:20pm</t>
+  </si>
+  <si>
+    <t>1:15pm</t>
+  </si>
+  <si>
+    <t>Working on Arithmetic Unit, trying to fix problems</t>
+  </si>
+  <si>
+    <t>1:30pm</t>
+  </si>
+  <si>
+    <t>4:17pm</t>
+  </si>
+  <si>
+    <t>Finished Arithmetic Unit and Logic Unit</t>
   </si>
 </sst>
 </file>
@@ -707,7 +716,7 @@
   <dimension ref="A1:G756"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -773,100 +782,120 @@
       <c r="B6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="9">
+        <v>43919</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="E6" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="12" t="s">
         <v>11</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="24.95" customHeight="1" thickBot="1">
       <c r="B7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>10</v>
+      <c r="C7" s="10">
+        <v>43919</v>
       </c>
       <c r="D7" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="G7" s="13" t="s">
         <v>15</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="24.95" customHeight="1" thickBot="1">
       <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="10">
+        <v>43920</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="13" t="s">
         <v>17</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="24.95" customHeight="1" thickBot="1">
       <c r="B9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>17</v>
+      <c r="C9" s="10">
+        <v>43920</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="24.95" customHeight="1" thickBot="1">
       <c r="B10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="10">
+        <v>43921</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="G10" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="24.95" customHeight="1" thickBot="1">
+      <c r="B11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="10">
+        <v>43922</v>
+      </c>
+      <c r="D11" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E11" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="24.95" customHeight="1" thickBot="1">
-      <c r="B11" s="12"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="22"/>
-      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="1:7" ht="24.95" customHeight="1">
-      <c r="B12" s="12"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="22"/>
-      <c r="G12" s="13"/>
+      <c r="B12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="10">
+        <v>43922</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="24.95" customHeight="1">
       <c r="B13" s="13"/>

</xml_diff>

<commit_message>
updated log and proofread documentation
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP1-log-G54-0624-350-1201.xlsx
+++ b/ExU/Documentation/FP1-log-G54-0624-350-1201.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rico\Desktop\ENSC 350 Part1\ENSC350FP\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F56E777-70AF-4B9D-B66B-8B48AA8317D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B446798-1E36-4F9A-AB72-253EE427B223}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5730" yWindow="3495" windowWidth="21600" windowHeight="11385" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -147,6 +147,15 @@
   </si>
   <si>
     <t>Continued with documentation and finished getting circuit screenshots, will try to finish up doucmentation tomorrow</t>
+  </si>
+  <si>
+    <t>7:25pm</t>
+  </si>
+  <si>
+    <t>7:41pm</t>
+  </si>
+  <si>
+    <t>Proofread the document once and made some changes, will submit tomorrow</t>
   </si>
 </sst>
 </file>
@@ -733,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD00F48-C874-4451-94D3-83F5136CE4E1}">
   <dimension ref="A1:G756"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -950,11 +959,21 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="24.95" customHeight="1">
-      <c r="B15" s="13"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="22"/>
-      <c r="G15" s="13"/>
+      <c r="B15" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="10">
+        <v>43925</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="24.95" customHeight="1">
       <c r="B16" s="13"/>

</xml_diff>